<commit_message>
Rasterdata from Pelletier and Plots
</commit_message>
<xml_diff>
--- a/analysis/tables/Landcover_Aridity_Comparison_Top10percent.xlsx
+++ b/analysis/tables/Landcover_Aridity_Comparison_Top10percent.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,15 +378,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Canopy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>WHC</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>High_Aridity</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>High_CTI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Sitename</t>
         </is>
@@ -404,13 +419,22 @@
       <c r="C2">
         <v>6.021</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>112.42</v>
+      </c>
+      <c r="F2">
+        <v>12.96</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>US-Cop</t>
         </is>
@@ -428,13 +452,22 @@
       <c r="C3">
         <v>5.134</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="D3">
+        <v>0.61</v>
+      </c>
+      <c r="E3">
+        <v>122.67</v>
+      </c>
+      <c r="F3">
+        <v>6.81</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>US-xNG</t>
         </is>
@@ -452,13 +485,22 @@
       <c r="C4">
         <v>4.151</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="D4">
+        <v>14.09</v>
+      </c>
+      <c r="E4">
+        <v>233.79</v>
+      </c>
+      <c r="F4">
+        <v>20.73</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>IL-Yat</t>
         </is>
@@ -476,13 +518,22 @@
       <c r="C5">
         <v>4.633</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="D5">
+        <v>1.35</v>
+      </c>
+      <c r="E5">
+        <v>111.3</v>
+      </c>
+      <c r="F5">
+        <v>13.46</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>US-xMB</t>
         </is>
@@ -500,13 +551,22 @@
       <c r="C6">
         <v>6.053</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="D6">
+        <v>1.35</v>
+      </c>
+      <c r="E6">
+        <v>129.52</v>
+      </c>
+      <c r="F6">
+        <v>19.65</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>US-Jo1</t>
         </is>
@@ -524,13 +584,22 @@
       <c r="C7">
         <v>4.261</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="D7">
+        <v>1.35</v>
+      </c>
+      <c r="E7">
+        <v>129.52</v>
+      </c>
+      <c r="F7">
+        <v>19.54</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>US-Jo2</t>
         </is>
@@ -548,13 +617,22 @@
       <c r="C8">
         <v>6.714</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>752.92</v>
+      </c>
+      <c r="F8">
+        <v>18.46</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>US-Tw4</t>
         </is>
@@ -572,13 +650,22 @@
       <c r="C9">
         <v>6.308</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+      <c r="E9">
+        <v>752.92</v>
+      </c>
+      <c r="F9">
+        <v>18.54</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>US-Tw3</t>
         </is>
@@ -596,13 +683,22 @@
       <c r="C10">
         <v>10.991</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>144.89</v>
+      </c>
+      <c r="F10">
+        <v>20.94</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>AU-GWW</t>
         </is>
@@ -620,13 +716,22 @@
       <c r="C11">
         <v>8.339</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>238.27</v>
+      </c>
+      <c r="F11">
+        <v>25.48</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>AU-Ync</t>
         </is>
@@ -644,13 +749,22 @@
       <c r="C12">
         <v>7.488</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="D12">
+        <v>6.5</v>
+      </c>
+      <c r="E12">
+        <v>149.11</v>
+      </c>
+      <c r="F12">
+        <v>25.48</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>AU-ASM</t>
         </is>
@@ -668,13 +782,22 @@
       <c r="C13">
         <v>6.335</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>141.82</v>
+      </c>
+      <c r="F13">
+        <v>20.71</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>AU-Cpr</t>
         </is>
@@ -692,13 +815,22 @@
       <c r="C14">
         <v>7.696</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="D14">
+        <v>0.47</v>
+      </c>
+      <c r="E14">
+        <v>1060.36</v>
+      </c>
+      <c r="F14">
+        <v>17.15</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>US-Sne</t>
         </is>
@@ -716,13 +848,22 @@
       <c r="C15">
         <v>4.876</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="D15">
+        <v>1.7</v>
+      </c>
+      <c r="E15">
+        <v>103.88</v>
+      </c>
+      <c r="F15">
+        <v>22.76</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>US-SRC</t>
         </is>
@@ -740,13 +881,22 @@
       <c r="C16">
         <v>4.396</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="D16">
+        <v>1.75</v>
+      </c>
+      <c r="E16">
+        <v>130.79</v>
+      </c>
+      <c r="F16">
+        <v>12.1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>US-xNQ</t>
         </is>
@@ -764,13 +914,22 @@
       <c r="C17">
         <v>4.878</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>129.52</v>
+      </c>
+      <c r="F17">
+        <v>20.5</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>US-Whs</t>
         </is>
@@ -788,13 +947,22 @@
       <c r="C18">
         <v>6.108</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>359</v>
+      </c>
+      <c r="F18">
+        <v>24.57</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>BW-Ma1</t>
         </is>
@@ -812,13 +980,22 @@
       <c r="C19">
         <v>5.212</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="D19">
+        <v>1.35</v>
+      </c>
+      <c r="E19">
+        <v>166.91</v>
+      </c>
+      <c r="F19">
+        <v>18.8</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>ES-Agu</t>
         </is>
@@ -836,13 +1013,22 @@
       <c r="C20">
         <v>4.733</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="D20">
+        <v>1.35</v>
+      </c>
+      <c r="E20">
+        <v>103.88</v>
+      </c>
+      <c r="F20">
+        <v>22.75</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>US-xSR</t>
         </is>
@@ -860,13 +1046,22 @@
       <c r="C21">
         <v>7.407</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="D21">
+        <v>2.05</v>
+      </c>
+      <c r="E21">
+        <v>731.26</v>
+      </c>
+      <c r="F21">
+        <v>17.59</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>US-Bi2</t>
         </is>
@@ -884,13 +1079,22 @@
       <c r="C22">
         <v>7.589</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="inlineStr">
+      <c r="D22">
+        <v>4.5</v>
+      </c>
+      <c r="E22">
+        <v>172.03</v>
+      </c>
+      <c r="F22">
+        <v>21.67</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>AR-SLu</t>
         </is>
@@ -908,13 +1112,22 @@
       <c r="C23">
         <v>6.533</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="D23">
+        <v>1.5</v>
+      </c>
+      <c r="E23">
+        <v>128.51</v>
+      </c>
+      <c r="F23">
+        <v>29.67</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>SD-Dem</t>
         </is>
@@ -932,13 +1145,22 @@
       <c r="C24">
         <v>4.497</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" t="inlineStr">
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>129.52</v>
+      </c>
+      <c r="F24">
+        <v>21.48</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>US-SRM</t>
         </is>
@@ -956,15 +1178,915 @@
       <c r="C25">
         <v>6.795</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="inlineStr">
+      <c r="D25">
+        <v>4.85</v>
+      </c>
+      <c r="E25">
+        <v>174.94</v>
+      </c>
+      <c r="F25">
+        <v>26.2</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>AU-TTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>4.81</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>6.784</v>
+      </c>
+      <c r="D26">
+        <v>12.44</v>
+      </c>
+      <c r="E26">
+        <v>209.92</v>
+      </c>
+      <c r="F26">
+        <v>6.28</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>US-xRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>4.518</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>4.447</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+      <c r="E27">
+        <v>129.52</v>
+      </c>
+      <c r="F27">
+        <v>19.42</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>US-Wkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>4.434</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>7.407</v>
+      </c>
+      <c r="D28">
+        <v>0.34</v>
+      </c>
+      <c r="E28">
+        <v>581.49</v>
+      </c>
+      <c r="F28">
+        <v>16.76</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>US-Bi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>4.305</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SAV</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>5.79</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>393.98</v>
+      </c>
+      <c r="F29">
+        <v>20.41</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>ES-Abr</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>4.302</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>7.407</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>778.42</v>
+      </c>
+      <c r="F30">
+        <v>17.17</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>US-Twt</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>4.224</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>EBF</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>5.111</v>
+      </c>
+      <c r="D31">
+        <v>28</v>
+      </c>
+      <c r="E31">
+        <v>196.98</v>
+      </c>
+      <c r="F31">
+        <v>16.71</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>AU-Whr</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>3.857</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>6.691</v>
+      </c>
+      <c r="D32">
+        <v>2.5</v>
+      </c>
+      <c r="E32">
+        <v>176.11</v>
+      </c>
+      <c r="F32">
+        <v>12.25</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>US-Ne3</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>3.749</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>6.121</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>180.19</v>
+      </c>
+      <c r="F33">
+        <v>21.29</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>US-SRG</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>3.578</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>4.629</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+      <c r="E34">
+        <v>359.49</v>
+      </c>
+      <c r="F34">
+        <v>14.08</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>AU-Otw</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>3.466</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>WSA</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>6.466</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>439.73</v>
+      </c>
+      <c r="F35">
+        <v>20.98</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>AU-Gin</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>3.317</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>6.691</v>
+      </c>
+      <c r="D36">
+        <v>2.5</v>
+      </c>
+      <c r="E36">
+        <v>180.27</v>
+      </c>
+      <c r="F36">
+        <v>12.15</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>US-Ne2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>3.283</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>WET</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>7.093</v>
+      </c>
+      <c r="D37">
+        <v>0.82</v>
+      </c>
+      <c r="E37">
+        <v>206.73</v>
+      </c>
+      <c r="F37">
+        <v>-0.71</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>US-BZB</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>3.223</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>EBF</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>4.935</v>
+      </c>
+      <c r="D38">
+        <v>40</v>
+      </c>
+      <c r="E38">
+        <v>504.65</v>
+      </c>
+      <c r="F38">
+        <v>10.5</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>AU-Tum</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>3.199</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>4.034</v>
+      </c>
+      <c r="D39">
+        <v>0.47</v>
+      </c>
+      <c r="E39">
+        <v>262.47</v>
+      </c>
+      <c r="F39">
+        <v>19.27</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>US-xCL</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>3.188</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>5.534</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>130.62</v>
+      </c>
+      <c r="F40">
+        <v>24.14</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>AU-Emr</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>3.161</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>7.126</v>
+      </c>
+      <c r="D41">
+        <v>0.4</v>
+      </c>
+      <c r="E41">
+        <v>196.72</v>
+      </c>
+      <c r="F41">
+        <v>17.42</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>AU-Rig</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>3.119</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>3.829</v>
+      </c>
+      <c r="D42">
+        <v>15.66</v>
+      </c>
+      <c r="E42">
+        <v>267.23</v>
+      </c>
+      <c r="F42">
+        <v>8.960000000000001</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>US-Me2</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>3.07</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>5.634</v>
+      </c>
+      <c r="D43">
+        <v>15.02</v>
+      </c>
+      <c r="E43">
+        <v>331.16</v>
+      </c>
+      <c r="F43">
+        <v>11.42</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>US-Fmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>3.032</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>6.66</v>
+      </c>
+      <c r="D44">
+        <v>0.75</v>
+      </c>
+      <c r="E44">
+        <v>154.81</v>
+      </c>
+      <c r="F44">
+        <v>7.84</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>CN-Cng</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>3.022</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>7.59</v>
+      </c>
+      <c r="D45">
+        <v>0.47</v>
+      </c>
+      <c r="E45">
+        <v>180.58</v>
+      </c>
+      <c r="F45">
+        <v>15.22</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>US-KLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>3.015</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WSA</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>5.323</v>
+      </c>
+      <c r="D46">
+        <v>7.1</v>
+      </c>
+      <c r="E46">
+        <v>365.86</v>
+      </c>
+      <c r="F46">
+        <v>18.53</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>US-Ton</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>2.962</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CSH</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>3.92</v>
+      </c>
+      <c r="D47">
+        <v>1.2</v>
+      </c>
+      <c r="E47">
+        <v>130.4</v>
+      </c>
+      <c r="F47">
+        <v>18.1</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>IT-Noe</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2.959</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>DBF</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>5.429</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+      <c r="E48">
+        <v>422.3</v>
+      </c>
+      <c r="F48">
+        <v>24.37</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>ZM-Mon</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>2.948</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CSH</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>2.785</v>
+      </c>
+      <c r="D49">
+        <v>1.6</v>
+      </c>
+      <c r="E49">
+        <v>252.39</v>
+      </c>
+      <c r="F49">
+        <v>6.59</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>US-Rms</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>2.88</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>5.08</v>
+      </c>
+      <c r="D50">
+        <v>1.18</v>
+      </c>
+      <c r="E50">
+        <v>154.61</v>
+      </c>
+      <c r="F50">
+        <v>11.21</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>US-xCP</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2.803</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>4.128</v>
+      </c>
+      <c r="D51">
+        <v>12.44</v>
+      </c>
+      <c r="E51">
+        <v>183.61</v>
+      </c>
+      <c r="F51">
+        <v>4.24</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>US-xYE</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>2.785</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>5.555</v>
+      </c>
+      <c r="D52">
+        <v>15.02</v>
+      </c>
+      <c r="E52">
+        <v>332.5</v>
+      </c>
+      <c r="F52">
+        <v>10.85</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>US-Fuf</t>
         </is>
       </c>
     </row>
@@ -975,7 +2097,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -999,15 +2121,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Canopy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>WHC</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>High_Aridity</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>High_CTI</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Sitename</t>
         </is>
@@ -1025,13 +2162,22 @@
       <c r="C2">
         <v>4.151</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D2">
+        <v>14.09</v>
+      </c>
+      <c r="E2">
+        <v>233.79</v>
+      </c>
+      <c r="F2">
+        <v>20.73</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>IL-Yat</t>
         </is>
@@ -1049,13 +2195,22 @@
       <c r="C3">
         <v>5.134</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="D3">
+        <v>0.61</v>
+      </c>
+      <c r="E3">
+        <v>122.67</v>
+      </c>
+      <c r="F3">
+        <v>6.81</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>US-xNG</t>
         </is>
@@ -1073,13 +2228,22 @@
       <c r="C4">
         <v>6.053</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="D4">
+        <v>1.35</v>
+      </c>
+      <c r="E4">
+        <v>129.52</v>
+      </c>
+      <c r="F4">
+        <v>19.65</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>US-Jo1</t>
         </is>
@@ -1097,13 +2261,22 @@
       <c r="C5">
         <v>6.714</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>752.92</v>
+      </c>
+      <c r="F5">
+        <v>18.46</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>US-Tw4</t>
         </is>
@@ -1121,13 +2294,22 @@
       <c r="C6">
         <v>4.633</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="D6">
+        <v>1.35</v>
+      </c>
+      <c r="E6">
+        <v>111.3</v>
+      </c>
+      <c r="F6">
+        <v>13.46</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>US-xMB</t>
         </is>
@@ -1145,13 +2327,22 @@
       <c r="C7">
         <v>4.733</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="D7">
+        <v>1.35</v>
+      </c>
+      <c r="E7">
+        <v>103.88</v>
+      </c>
+      <c r="F7">
+        <v>22.75</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>US-xSR</t>
         </is>
@@ -1169,13 +2360,22 @@
       <c r="C8">
         <v>4.396</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="D8">
+        <v>1.75</v>
+      </c>
+      <c r="E8">
+        <v>130.79</v>
+      </c>
+      <c r="F8">
+        <v>12.1</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>US-xNQ</t>
         </is>
@@ -1193,13 +2393,22 @@
       <c r="C9">
         <v>6.784</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="D9">
+        <v>12.44</v>
+      </c>
+      <c r="E9">
+        <v>209.92</v>
+      </c>
+      <c r="F9">
+        <v>6.28</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>US-xRM</t>
         </is>
@@ -1217,13 +2426,22 @@
       <c r="C10">
         <v>5.212</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="inlineStr">
+      <c r="D10">
+        <v>1.35</v>
+      </c>
+      <c r="E10">
+        <v>166.91</v>
+      </c>
+      <c r="F10">
+        <v>18.8</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>ES-Agu</t>
         </is>
@@ -1241,13 +2459,22 @@
       <c r="C11">
         <v>8.339</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>238.27</v>
+      </c>
+      <c r="F11">
+        <v>25.48</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>AU-Ync</t>
         </is>
@@ -1265,13 +2492,22 @@
       <c r="C12">
         <v>7.488</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="D12">
+        <v>6.5</v>
+      </c>
+      <c r="E12">
+        <v>149.11</v>
+      </c>
+      <c r="F12">
+        <v>25.48</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>AU-ASM</t>
         </is>
@@ -1289,13 +2525,22 @@
       <c r="C13">
         <v>6.108</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>359</v>
+      </c>
+      <c r="F13">
+        <v>24.57</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>BW-Ma1</t>
         </is>
@@ -1313,13 +2558,22 @@
       <c r="C14">
         <v>4.261</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="D14">
+        <v>1.35</v>
+      </c>
+      <c r="E14">
+        <v>129.52</v>
+      </c>
+      <c r="F14">
+        <v>19.54</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>US-Jo2</t>
         </is>
@@ -1337,13 +2591,22 @@
       <c r="C15">
         <v>5.79</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>393.98</v>
+      </c>
+      <c r="F15">
+        <v>20.41</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>ES-Abr</t>
         </is>
@@ -1361,13 +2624,22 @@
       <c r="C16">
         <v>7.696</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="D16">
+        <v>0.47</v>
+      </c>
+      <c r="E16">
+        <v>1060.36</v>
+      </c>
+      <c r="F16">
+        <v>17.15</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>US-Sne</t>
         </is>
@@ -1385,13 +2657,22 @@
       <c r="C17">
         <v>10.991</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="inlineStr">
+      <c r="D17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>144.89</v>
+      </c>
+      <c r="F17">
+        <v>20.94</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>AU-GWW</t>
         </is>
@@ -1409,13 +2690,22 @@
       <c r="C18">
         <v>6.021</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>112.42</v>
+      </c>
+      <c r="F18">
+        <v>12.96</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>US-Cop</t>
         </is>
@@ -1433,13 +2723,22 @@
       <c r="C19">
         <v>7.407</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="D19">
+        <v>2.05</v>
+      </c>
+      <c r="E19">
+        <v>731.26</v>
+      </c>
+      <c r="F19">
+        <v>17.59</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>US-Bi2</t>
         </is>
@@ -1457,13 +2756,22 @@
       <c r="C20">
         <v>4.034</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="D20">
+        <v>0.47</v>
+      </c>
+      <c r="E20">
+        <v>262.47</v>
+      </c>
+      <c r="F20">
+        <v>19.27</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>US-xCL</t>
         </is>
@@ -1481,13 +2789,22 @@
       <c r="C21">
         <v>6.308</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="D21">
+        <v>0.3</v>
+      </c>
+      <c r="E21">
+        <v>752.92</v>
+      </c>
+      <c r="F21">
+        <v>18.54</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>US-Tw3</t>
         </is>
@@ -1505,13 +2822,22 @@
       <c r="C22">
         <v>6.795</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr">
+      <c r="D22">
+        <v>4.85</v>
+      </c>
+      <c r="E22">
+        <v>174.94</v>
+      </c>
+      <c r="F22">
+        <v>26.2</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>AU-TTE</t>
         </is>
@@ -1529,13 +2855,22 @@
       <c r="C23">
         <v>7.589</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="D23">
+        <v>4.5</v>
+      </c>
+      <c r="E23">
+        <v>172.03</v>
+      </c>
+      <c r="F23">
+        <v>21.67</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>AR-SLu</t>
         </is>
@@ -1553,13 +2888,22 @@
       <c r="C24">
         <v>6.335</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" t="inlineStr">
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>141.82</v>
+      </c>
+      <c r="F24">
+        <v>20.71</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>AU-Cpr</t>
         </is>
@@ -1577,15 +2921,882 @@
       <c r="C25">
         <v>4.876</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="inlineStr">
+      <c r="D25">
+        <v>1.7</v>
+      </c>
+      <c r="E25">
+        <v>103.88</v>
+      </c>
+      <c r="F25">
+        <v>22.76</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>US-SRC</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2.252</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>5.634</v>
+      </c>
+      <c r="D26">
+        <v>15.02</v>
+      </c>
+      <c r="E26">
+        <v>331.16</v>
+      </c>
+      <c r="F26">
+        <v>11.42</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>US-Fmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2.227</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>7.407</v>
+      </c>
+      <c r="D27">
+        <v>0.34</v>
+      </c>
+      <c r="E27">
+        <v>581.49</v>
+      </c>
+      <c r="F27">
+        <v>16.76</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>US-Bi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2.212</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>OSH</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>4.878</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>129.52</v>
+      </c>
+      <c r="F28">
+        <v>20.5</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>US-Whs</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2.209</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>WSA</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>4.497</v>
+      </c>
+      <c r="D29">
+        <v>2.5</v>
+      </c>
+      <c r="E29">
+        <v>129.52</v>
+      </c>
+      <c r="F29">
+        <v>21.48</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>US-SRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2.185</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>EBF</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>5.111</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>196.98</v>
+      </c>
+      <c r="F30">
+        <v>16.71</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>AU-Whr</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>2.126</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>WSA</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>6.466</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>439.73</v>
+      </c>
+      <c r="F31">
+        <v>20.98</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>AU-Gin</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2.092</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>7.407</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>778.42</v>
+      </c>
+      <c r="F32">
+        <v>17.17</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>US-Twt</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2.075</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>5.555</v>
+      </c>
+      <c r="D33">
+        <v>15.02</v>
+      </c>
+      <c r="E33">
+        <v>332.5</v>
+      </c>
+      <c r="F33">
+        <v>10.85</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>US-Fuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>2.062</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SAV</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>6.533</v>
+      </c>
+      <c r="D34">
+        <v>1.5</v>
+      </c>
+      <c r="E34">
+        <v>128.51</v>
+      </c>
+      <c r="F34">
+        <v>29.67</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>SD-Dem</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2.056</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>4.128</v>
+      </c>
+      <c r="D35">
+        <v>12.44</v>
+      </c>
+      <c r="E35">
+        <v>183.61</v>
+      </c>
+      <c r="F35">
+        <v>4.24</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>US-xYE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>1.987</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SAV</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>5.442</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>341.99</v>
+      </c>
+      <c r="F36">
+        <v>19.5</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>ES-LM2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>1.966</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>4.447</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+      <c r="E37">
+        <v>129.52</v>
+      </c>
+      <c r="F37">
+        <v>19.42</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>US-Wkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>1.959</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>5.08</v>
+      </c>
+      <c r="D38">
+        <v>1.18</v>
+      </c>
+      <c r="E38">
+        <v>154.61</v>
+      </c>
+      <c r="F38">
+        <v>11.21</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>US-xCP</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>1.945</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>5.534</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>130.62</v>
+      </c>
+      <c r="F39">
+        <v>24.14</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>AU-Emr</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>1.936</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>6.691</v>
+      </c>
+      <c r="D40">
+        <v>2.5</v>
+      </c>
+      <c r="E40">
+        <v>176.11</v>
+      </c>
+      <c r="F40">
+        <v>12.25</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>US-Ne3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>1.909</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SAV</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>5.442</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>341.99</v>
+      </c>
+      <c r="F41">
+        <v>19.41</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ES-LM1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>1.899</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>5.319</v>
+      </c>
+      <c r="D42">
+        <v>0.61</v>
+      </c>
+      <c r="E42">
+        <v>180.3</v>
+      </c>
+      <c r="F42">
+        <v>5.6</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>US-xDC</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1.86</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>EBF</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>4.935</v>
+      </c>
+      <c r="D43">
+        <v>40</v>
+      </c>
+      <c r="E43">
+        <v>504.65</v>
+      </c>
+      <c r="F43">
+        <v>10.5</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>AU-Tum</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>1.844</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DBF</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>5.429</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>422.3</v>
+      </c>
+      <c r="F44">
+        <v>24.37</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>ZM-Mon</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>1.839</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>6.691</v>
+      </c>
+      <c r="D45">
+        <v>2.5</v>
+      </c>
+      <c r="E45">
+        <v>180.27</v>
+      </c>
+      <c r="F45">
+        <v>12.15</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>US-Ne2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>1.828</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>4.629</v>
+      </c>
+      <c r="D46">
+        <v>0.1</v>
+      </c>
+      <c r="E46">
+        <v>359.49</v>
+      </c>
+      <c r="F46">
+        <v>14.08</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>AU-Otw</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>1.818</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>4.456</v>
+      </c>
+      <c r="D47">
+        <v>0.47</v>
+      </c>
+      <c r="E47">
+        <v>188.92</v>
+      </c>
+      <c r="F47">
+        <v>13.95</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>US-xKZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>1.804</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>3.829</v>
+      </c>
+      <c r="D48">
+        <v>15.66</v>
+      </c>
+      <c r="E48">
+        <v>267.23</v>
+      </c>
+      <c r="F48">
+        <v>8.960000000000001</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>US-Me2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>1.804</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>WSA</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>5.101</v>
+      </c>
+      <c r="D49">
+        <v>2.5</v>
+      </c>
+      <c r="E49">
+        <v>488.82</v>
+      </c>
+      <c r="F49">
+        <v>19.64</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>ES-Cnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>1.791</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>GRA</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>6.121</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>180.19</v>
+      </c>
+      <c r="F50">
+        <v>21.29</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>US-SRG</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>1.779</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ENF</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>4.479</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>887.16</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>CA-SF1</t>
         </is>
       </c>
     </row>
@@ -1596,7 +3807,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1622,105 +3833,144 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OSH</t>
+          <t>GRA</t>
         </is>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>33.3</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GRA</t>
+          <t>OSH</t>
         </is>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>20.8</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SAV</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>20.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>ENF</t>
         </is>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>8.300000000000001</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ENF</t>
+          <t>SAV</t>
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>4.2</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MF</t>
+          <t>WSA</t>
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>4.2</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WET</t>
+          <t>CSH</t>
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>4.2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WSA</t>
+          <t>EBF</t>
         </is>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>4.2</v>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WET</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DBF</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MF</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1730,7 +3980,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1756,14 +4006,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OSH</t>
+          <t>ENF</t>
         </is>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>29.2</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="3">
@@ -1773,75 +4023,114 @@
         </is>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SAV</t>
+          <t>OSH</t>
         </is>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>20.8</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>SAV</t>
         </is>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>8.300000000000001</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ENF</t>
+          <t>CRO</t>
         </is>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>8.300000000000001</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MF</t>
+          <t>WSA</t>
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>4.2</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>EBF</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DBF</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MF</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>WET</t>
         </is>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>4.2</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>